<commit_message>
fixing the SRS req 13 in RTM based on the review point
</commit_message>
<xml_diff>
--- a/SWE/SW deliveries log/RTM/RTM.xlsx
+++ b/SWE/SW deliveries log/RTM/RTM.xlsx
@@ -404,37 +404,16 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -449,14 +428,41 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -466,12 +472,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -695,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -723,7 +723,7 @@
       <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="2"/>
@@ -750,16 +750,16 @@
     </row>
     <row r="2" spans="1:26" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="8"/>
@@ -786,10 +786,10 @@
     </row>
     <row r="3" spans="1:26" s="6" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="25" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="19" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="8"/>
@@ -816,10 +816,10 @@
     </row>
     <row r="4" spans="1:26" s="6" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="24" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="18" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="8"/>
@@ -846,10 +846,10 @@
     </row>
     <row r="5" spans="1:26" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="25" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="19" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="8"/>
@@ -876,10 +876,10 @@
     </row>
     <row r="6" spans="1:26" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="24" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="18" t="s">
         <v>26</v>
       </c>
       <c r="F6" s="8"/>
@@ -906,9 +906,9 @@
     </row>
     <row r="7" spans="1:26" s="6" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="9" t="s">
         <v>27</v>
       </c>
@@ -936,7 +936,7 @@
     </row>
     <row r="8" spans="1:26" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="23"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="14" t="s">
         <v>56</v>
       </c>
@@ -968,7 +968,7 @@
     </row>
     <row r="9" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -977,7 +977,7 @@
       <c r="D9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="7"/>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="10" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10" s="21"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="14" t="s">
         <v>7</v>
       </c>
@@ -1038,14 +1038,16 @@
     </row>
     <row r="11" spans="1:26" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1070,8 +1072,8 @@
     </row>
     <row r="12" spans="1:26" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="30"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
@@ -1100,8 +1102,8 @@
     </row>
     <row r="13" spans="1:26" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="38"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="14" t="s">
         <v>12</v>
       </c>
@@ -1130,8 +1132,8 @@
     </row>
     <row r="14" spans="1:26" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="38"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="14" t="s">
         <v>64</v>
       </c>
@@ -1160,8 +1162,8 @@
     </row>
     <row r="15" spans="1:26" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="38"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="14" t="s">
         <v>65</v>
       </c>
@@ -1190,10 +1192,10 @@
     </row>
     <row r="16" spans="1:26" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -1226,16 +1228,16 @@
     </row>
     <row r="17" spans="1:26" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="37" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="32" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="2"/>
@@ -1262,12 +1264,12 @@
     </row>
     <row r="18" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="36"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="21"/>
+      <c r="E18" s="32"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1292,8 +1294,8 @@
     </row>
     <row r="19" spans="1:26" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="36"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="38"/>
       <c r="D19" s="12" t="s">
         <v>11</v>
       </c>
@@ -1322,12 +1324,12 @@
     </row>
     <row r="20" spans="1:26" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="36"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="2"/>
@@ -1354,12 +1356,12 @@
     </row>
     <row r="21" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="36"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="38"/>
       <c r="D21" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="21"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1384,14 +1386,14 @@
     </row>
     <row r="22" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="32" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="13"/>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="21" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="2"/>
@@ -1418,8 +1420,8 @@
     </row>
     <row r="23" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="21"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="13"/>
       <c r="E23" s="15" t="s">
         <v>34</v>
@@ -1448,10 +1450,10 @@
     </row>
     <row r="24" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="21"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="13"/>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="21" t="s">
         <v>35</v>
       </c>
       <c r="F24" s="2"/>
@@ -1478,8 +1480,8 @@
     </row>
     <row r="25" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="13"/>
       <c r="E25" s="15" t="s">
         <v>36</v>
@@ -1508,10 +1510,10 @@
     </row>
     <row r="26" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="21"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F26" s="2"/>
@@ -1538,8 +1540,8 @@
     </row>
     <row r="27" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="13"/>
       <c r="E27" s="15" t="s">
         <v>38</v>
@@ -1568,10 +1570,10 @@
     </row>
     <row r="28" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="21"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="21" t="s">
         <v>48</v>
       </c>
       <c r="F28" s="2"/>
@@ -1598,10 +1600,10 @@
     </row>
     <row r="29" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="26" t="s">
         <v>51</v>
       </c>
       <c r="D29" s="13"/>
@@ -1630,13 +1632,17 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="37"/>
+      <c r="B30" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="D30" s="13"/>
-      <c r="E30" s="13" t="s">
-        <v>33</v>
+      <c r="E30" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1660,18 +1666,16 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
-    <row r="31" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" s="6" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="15" t="s">
-        <v>55</v>
+      <c r="B31" s="21" t="s">
+        <v>57</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>47</v>
+      <c r="C31" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="D31" s="13"/>
-      <c r="E31" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="E31" s="15"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1694,16 +1698,16 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
     </row>
-    <row r="32" spans="1:26" s="6" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="28" t="s">
-        <v>57</v>
+      <c r="B32" s="28"/>
+      <c r="C32" s="29" t="s">
+        <v>50</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>58</v>
+      <c r="D32" s="28"/>
+      <c r="E32" s="13" t="s">
+        <v>31</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="15"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1726,15 +1730,13 @@
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
     </row>
-    <row r="33" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="31"/>
-      <c r="E33" s="13" t="s">
-        <v>31</v>
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -1758,13 +1760,15 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
     </row>
-    <row r="34" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="15" t="s">
-        <v>42</v>
+      <c r="B34" s="28"/>
+      <c r="C34" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="28"/>
+      <c r="E34" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -1788,15 +1792,15 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
     </row>
-    <row r="35" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="32" t="s">
-        <v>44</v>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29" t="s">
+        <v>45</v>
       </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="22" t="s">
-        <v>43</v>
+      <c r="D35" s="28"/>
+      <c r="E35" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -1820,15 +1824,13 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
     </row>
-    <row r="36" spans="1:26" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="31"/>
-      <c r="E36" s="15" t="s">
-        <v>32</v>
+      <c r="B36" s="28"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1852,14 +1854,14 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
-    <row r="37" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="13" t="s">
-        <v>41</v>
+      <c r="B37" s="28"/>
+      <c r="C37" s="22" t="s">
+        <v>18</v>
       </c>
+      <c r="D37" s="28"/>
+      <c r="E37" s="15"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -1882,14 +1884,12 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
     </row>
-    <row r="38" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="31"/>
-      <c r="E38" s="15"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -1912,7 +1912,7 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
     </row>
-    <row r="39" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="2"/>
@@ -28820,53 +28820,23 @@
       <c r="Y999" s="2"/>
       <c r="Z999" s="2"/>
     </row>
-    <row r="1000" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1000" s="4"/>
-      <c r="B1000" s="5"/>
-      <c r="C1000" s="2"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="2"/>
-      <c r="F1000" s="2"/>
-      <c r="G1000" s="2"/>
-      <c r="H1000" s="2"/>
-      <c r="I1000" s="2"/>
-      <c r="J1000" s="2"/>
-      <c r="K1000" s="2"/>
-      <c r="L1000" s="2"/>
-      <c r="M1000" s="2"/>
-      <c r="N1000" s="2"/>
-      <c r="O1000" s="2"/>
-      <c r="P1000" s="2"/>
-      <c r="Q1000" s="2"/>
-      <c r="R1000" s="2"/>
-      <c r="S1000" s="2"/>
-      <c r="T1000" s="2"/>
-      <c r="U1000" s="2"/>
-      <c r="V1000" s="2"/>
-      <c r="W1000" s="2"/>
-      <c r="X1000" s="2"/>
-      <c r="Y1000" s="2"/>
-      <c r="Z1000" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D38"/>
-    <mergeCell ref="C36:C37"/>
+  <mergeCells count="15">
     <mergeCell ref="B22:B28"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="C22:C28"/>
-    <mergeCell ref="C29:C30"/>
     <mergeCell ref="C2:C7"/>
     <mergeCell ref="D2:D7"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="C17:C21"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D37"/>
+    <mergeCell ref="C35:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>